<commit_message>
Added most of Paden's code
Added a lot of Paden's code into Master Branch
</commit_message>
<xml_diff>
--- a/Zeus/data/TSP/Problems/bays29.xlsx
+++ b/Zeus/data/TSP/Problems/bays29.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlm1026\Desktop\ToAdd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dds1010\Desktop\full-matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>NAME</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>EDGE_WEIGHT_SECTION</t>
-  </si>
-  <si>
-    <t>DISPLAY_DATA_SECTION</t>
   </si>
   <si>
     <t>EOF</t>
@@ -445,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC67"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,330 +3116,6 @@
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38">
-        <v>1150</v>
-      </c>
-      <c r="C38">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39">
-        <v>630</v>
-      </c>
-      <c r="C39">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40">
-        <v>40</v>
-      </c>
-      <c r="C40">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>4</v>
-      </c>
-      <c r="B41">
-        <v>750</v>
-      </c>
-      <c r="C41">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>750</v>
-      </c>
-      <c r="C42">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>6</v>
-      </c>
-      <c r="B43">
-        <v>1030</v>
-      </c>
-      <c r="C43">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>7</v>
-      </c>
-      <c r="B44">
-        <v>1650</v>
-      </c>
-      <c r="C44">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>1490</v>
-      </c>
-      <c r="C45">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>790</v>
-      </c>
-      <c r="C46">
-        <v>2260</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>710</v>
-      </c>
-      <c r="C47">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>11</v>
-      </c>
-      <c r="B48">
-        <v>840</v>
-      </c>
-      <c r="C48">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>12</v>
-      </c>
-      <c r="B49">
-        <v>1170</v>
-      </c>
-      <c r="C49">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>13</v>
-      </c>
-      <c r="B50">
-        <v>970</v>
-      </c>
-      <c r="C50">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>14</v>
-      </c>
-      <c r="B51">
-        <v>510</v>
-      </c>
-      <c r="C51">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>15</v>
-      </c>
-      <c r="B52">
-        <v>750</v>
-      </c>
-      <c r="C52">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>16</v>
-      </c>
-      <c r="B53">
-        <v>1280</v>
-      </c>
-      <c r="C53">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>17</v>
-      </c>
-      <c r="B54">
-        <v>230</v>
-      </c>
-      <c r="C54">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>18</v>
-      </c>
-      <c r="B55">
-        <v>460</v>
-      </c>
-      <c r="C55">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>19</v>
-      </c>
-      <c r="B56">
-        <v>1040</v>
-      </c>
-      <c r="C56">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>20</v>
-      </c>
-      <c r="B57">
-        <v>590</v>
-      </c>
-      <c r="C57">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>21</v>
-      </c>
-      <c r="B58">
-        <v>830</v>
-      </c>
-      <c r="C58">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>22</v>
-      </c>
-      <c r="B59">
-        <v>490</v>
-      </c>
-      <c r="C59">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>23</v>
-      </c>
-      <c r="B60">
-        <v>1840</v>
-      </c>
-      <c r="C60">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>24</v>
-      </c>
-      <c r="B61">
-        <v>1260</v>
-      </c>
-      <c r="C61">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>25</v>
-      </c>
-      <c r="B62">
-        <v>1280</v>
-      </c>
-      <c r="C62">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>26</v>
-      </c>
-      <c r="B63">
-        <v>490</v>
-      </c>
-      <c r="C63">
-        <v>2130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>27</v>
-      </c>
-      <c r="B64">
-        <v>1460</v>
-      </c>
-      <c r="C64">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>28</v>
-      </c>
-      <c r="B65">
-        <v>1260</v>
-      </c>
-      <c r="C65">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>29</v>
-      </c>
-      <c r="B66">
-        <v>360</v>
-      </c>
-      <c r="C66">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>